<commit_message>
remove score from tables
</commit_message>
<xml_diff>
--- a/tables/Fulcrum.xlsx
+++ b/tables/Fulcrum.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KAlstad\Documents\Github_C\e-device2\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KAlstad\Documents\Github_C\e-deviceIEP\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2240A37-2767-4E4C-9ECC-8AA299B0D01D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75034CF5-39B2-47B8-A43E-FFACDCD0AC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E4A5BE10-DBB8-481B-874B-1BDF43DE8625}"/>
+    <workbookView xWindow="29580" yWindow="975" windowWidth="27960" windowHeight="11385" xr2:uid="{E4A5BE10-DBB8-481B-874B-1BDF43DE8625}"/>
   </bookViews>
   <sheets>
     <sheet name="Forms_Options" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="114">
   <si>
     <t>Feature</t>
   </si>
@@ -435,16 +435,10 @@
     <t>Group</t>
   </si>
   <si>
-    <t>Score</t>
-  </si>
-  <si>
     <t>Group Notes/Reviews</t>
   </si>
   <si>
     <t>External Reviews</t>
-  </si>
-  <si>
-    <t>Score (0-3)</t>
   </si>
   <si>
     <t>Cloud-storage</t>
@@ -639,7 +633,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -685,14 +679,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF202124"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -775,9 +761,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -788,7 +774,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -797,22 +783,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -827,16 +810,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -845,8 +828,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1169,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FEDC525-B77D-4397-8B91-1C5526620A5B}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="105" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1168,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -1204,11 +1187,8 @@
       <c r="F1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -1216,13 +1196,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -1230,13 +1210,13 @@
         <v>47</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -1244,14 +1224,14 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="F4"/>
     </row>
-    <row r="5" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
@@ -1259,13 +1239,13 @@
         <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
@@ -1273,13 +1253,13 @@
         <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -1287,16 +1267,16 @@
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -1304,30 +1284,30 @@
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1335,17 +1315,17 @@
         <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" s="18"/>
-    </row>
-    <row r="11" spans="1:7" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -1353,14 +1333,14 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F11"/>
     </row>
-    <row r="12" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -1368,13 +1348,13 @@
         <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -1382,7 +1362,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -1390,16 +1370,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="17"/>
-    </row>
-    <row r="16" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="16"/>
+    </row>
+    <row r="16" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
@@ -1426,10 +1406,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C0BCC4-86A1-4030-90CE-22D0CC9ADA23}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,12 +1418,11 @@
     <col min="4" max="4" width="41.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="71" style="1" customWidth="1"/>
     <col min="6" max="6" width="27.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="46.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="21.85546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -1457,44 +1436,41 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -1504,21 +1480,20 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:8" s="5" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="5" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="E6" s="14"/>
+      <c r="D6" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="13"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>42</v>
       </c>
@@ -1529,10 +1504,9 @@
       <c r="D7" s="5"/>
       <c r="E7" s="7"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
@@ -1540,9 +1514,8 @@
         <v>15</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
@@ -1550,9 +1523,8 @@
         <v>16</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -1560,10 +1532,10 @@
         <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1574,10 +1546,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF5D6FA-27AF-4377-9AE3-FE0575D1CE52}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1585,10 +1557,9 @@
     <col min="1" max="4" width="35.140625" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -1602,16 +1573,13 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s">
         <v>64</v>
       </c>
-      <c r="F1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" s="5" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>48</v>
       </c>
@@ -1619,23 +1587,23 @@
         <v>20</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="5" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="20"/>
-      <c r="F3" s="11"/>
-    </row>
-    <row r="4" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1643,11 +1611,11 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1655,15 +1623,15 @@
         <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="F5" s="22"/>
-    </row>
-    <row r="6" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="21"/>
+    </row>
+    <row r="6" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>45</v>
       </c>
@@ -1671,26 +1639,25 @@
         <v>49</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:7" ht="174.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="174.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -1698,16 +1665,16 @@
         <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1718,10 +1685,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6FF90FC-7D54-4396-BEBF-836B30C262EA}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,11 +1697,10 @@
     <col min="2" max="2" width="44.5703125" style="5" customWidth="1"/>
     <col min="3" max="3" width="26.85546875" style="5" customWidth="1"/>
     <col min="4" max="4" width="23" style="5" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="5"/>
+    <col min="5" max="5" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>50</v>
       </c>
@@ -1742,64 +1708,61 @@
         <v>57</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="16"/>
-    </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="B2" s="15"/>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>55</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
         <v>56</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
         <v>59</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
         <v>58</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1810,10 +1773,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C265533-1A49-4A12-B530-D6DEC4C9BC87}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1825,7 +1788,7 @@
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1836,66 +1799,63 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
         <v>64</v>
       </c>
-      <c r="E1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>98</v>
+      <c r="B2" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="11"/>
-    </row>
-    <row r="4" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="13"/>
-    </row>
-    <row r="5" spans="1:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="C4" s="12"/>
+    </row>
+    <row r="5" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C5" s="13"/>
-    </row>
-    <row r="6" spans="1:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:5" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="D6" s="13"/>
+        <v>101</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1905,10 +1865,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DAF0C1-5840-4498-93BE-7596EB0B3995}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1918,10 +1878,9 @@
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="31.42578125" customWidth="1"/>
     <col min="5" max="5" width="46.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1929,96 +1888,89 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="F1" s="5"/>
       <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>51</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E9" s="23"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>